<commit_message>
Update with report html file
</commit_message>
<xml_diff>
--- a/src/main/java/FrameworkApp/Sample/Data/Actitime.xlsx
+++ b/src/main/java/FrameworkApp/Sample/Data/Actitime.xlsx
@@ -69,10 +69,10 @@
     <t>Username or Password is invalid. Please try again.</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
     <t>Logout</t>
-  </si>
-  <si>
-    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -437,7 +439,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -508,7 +510,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>